<commit_message>
🔄 Mise à jour des fichiers Excel et du script generate_charts.py
</commit_message>
<xml_diff>
--- a/CDD/Data temperatures.xlsx
+++ b/CDD/Data temperatures.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\gvaps1\USR6\CHGE\desktop\Fuel desk\CDD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\gvaps1\USR6\CHGE\desktop\Fuel dashboard\CDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91D3B1C-F80C-4929-BE0E-5ABEB11E4FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12301EF1-FF16-45ED-8E07-43210E8C27C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{805FC610-D0B7-4151-AF7A-494C14C34CCD}"/>
   </bookViews>
@@ -485,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF6C800-FC25-4C64-B3CE-5880A9630BFD}">
-  <dimension ref="A1:E2036"/>
+  <dimension ref="A1:E2039"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2012" workbookViewId="0">
-      <selection activeCell="L2033" sqref="L2033"/>
+    <sheetView tabSelected="1" topLeftCell="A2018" workbookViewId="0">
+      <selection activeCell="F2047" sqref="F2047"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,14 +550,14 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","Per=D","Days=A","Dts=S","cols=2;rows=2030")</f>
+        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","Per=D","Days=A","Dts=S","cols=2;rows=2033")</f>
         <v>43831</v>
       </c>
       <c r="B7">
         <v>13.43</v>
       </c>
       <c r="C7">
-        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","Per=D","Days=A","Dts=H","cols=1;rows=2030")</f>
+        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","Per=D","Days=A","Dts=H","cols=1;rows=2033")</f>
         <v>18.16</v>
       </c>
       <c r="D7">
@@ -38865,7 +38865,7 @@
         <v>35.93</v>
       </c>
       <c r="D2023">
-        <f t="shared" ref="D2023:E2036" si="56">IF(B2023&gt;18,1,0)</f>
+        <f t="shared" ref="D2023:E2038" si="56">IF(B2023&gt;18,1,0)</f>
         <v>1</v>
       </c>
       <c r="E2023">
@@ -39087,10 +39087,10 @@
         <v>45859</v>
       </c>
       <c r="B2035">
-        <v>29.32</v>
+        <v>29.9</v>
       </c>
       <c r="C2035">
-        <v>37.049999999999997</v>
+        <v>37.11</v>
       </c>
       <c r="D2035">
         <f t="shared" si="56"/>
@@ -39106,10 +39106,10 @@
         <v>45860</v>
       </c>
       <c r="B2036">
-        <v>29.32</v>
+        <v>30.28</v>
       </c>
       <c r="C2036">
-        <v>37.049999999999997</v>
+        <v>37.68</v>
       </c>
       <c r="D2036">
         <f t="shared" si="56"/>
@@ -39117,6 +39117,63 @@
       </c>
       <c r="E2036">
         <f t="shared" si="56"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2037" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2037" s="2">
+        <v>45861</v>
+      </c>
+      <c r="B2037">
+        <v>31.57</v>
+      </c>
+      <c r="C2037">
+        <v>37.840000000000003</v>
+      </c>
+      <c r="D2037">
+        <f t="shared" si="56"/>
+        <v>1</v>
+      </c>
+      <c r="E2037">
+        <f t="shared" si="56"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2038" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2038" s="2">
+        <v>45862</v>
+      </c>
+      <c r="B2038">
+        <v>31.57</v>
+      </c>
+      <c r="C2038">
+        <v>37.840000000000003</v>
+      </c>
+      <c r="D2038">
+        <f t="shared" si="56"/>
+        <v>1</v>
+      </c>
+      <c r="E2038">
+        <f t="shared" si="56"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2039" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2039" s="2">
+        <v>45863</v>
+      </c>
+      <c r="B2039">
+        <v>31.57</v>
+      </c>
+      <c r="C2039">
+        <v>37.840000000000003</v>
+      </c>
+      <c r="D2039">
+        <f t="shared" ref="D2039:E2039" si="57">IF(B2039&gt;18,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E2039">
+        <f t="shared" si="57"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>